<commit_message>
added Bank power info to XLS
</commit_message>
<xml_diff>
--- a/0.doc/CRUVI-camera-adapter/CRUVI-Pinout-4-and-2-lanes.xlsx
+++ b/0.doc/CRUVI-camera-adapter/CRUVI-Pinout-4-and-2-lanes.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="396" yWindow="312" windowWidth="15012" windowHeight="8220"/>
+    <workbookView xWindow="400" yWindow="310" windowWidth="15010" windowHeight="8220" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="4 Lanes" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="130">
   <si>
     <t>pin</t>
   </si>
@@ -489,6 +489,44 @@
 1) Camera I2C is kept separately from I2C for CRUVI-optional ID EEPROM
 2) Pay attention to voltage levels between FPGA (VADJ) and Camera I2C and POWER_EN, which are 3.3V</t>
     </r>
+  </si>
+  <si>
+    <t>VCCIO35</t>
+  </si>
+  <si>
+    <t>VCCIO_CA</t>
+  </si>
+  <si>
+    <t>VCCIO15</t>
+  </si>
+  <si>
+    <t>VCCIO_CC</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>VS0, 1, 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> come from CPLD. Default RTL provides 1.8V and 2.5V:</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">FPGA IBUFDS, to be LVDS, can only work with 2.5V (LVDS_25) and 1.8V VCCO (LVDS) </t>
   </si>
 </sst>
 </file>
@@ -1242,9 +1280,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1281,31 +1316,7 @@
     <xf numFmtId="0" fontId="23" fillId="37" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1322,9 +1333,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1360,59 +1368,89 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1466,6 +1504,396 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>311150</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>6766</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2552700" y="5683249"/>
+          <a:ext cx="1504950" cy="1441867"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>533662</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>158781</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="628650" y="7226300"/>
+          <a:ext cx="5099312" cy="603281"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>768541</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>44550</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="806450" y="7988300"/>
+          <a:ext cx="3708591" cy="1936850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>603250</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>216100</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>171565</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="889000" y="10388600"/>
+          <a:ext cx="3899100" cy="2241665"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>965200</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>25530</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>76</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1250950" y="13328650"/>
+          <a:ext cx="2521080" cy="1479626"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>222250</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>603250</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>132260</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2120900" y="4552950"/>
+          <a:ext cx="1714500" cy="1592760"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>120650</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>876562</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>158781</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="482600" y="6305550"/>
+          <a:ext cx="5099312" cy="603281"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>82741</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>120750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1079500" y="6959600"/>
+          <a:ext cx="3708591" cy="1936850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>654050</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>209750</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>114415</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1016000" y="9226550"/>
+          <a:ext cx="3899100" cy="2241665"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>44450</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>685930</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>76</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1397000" y="12039600"/>
+          <a:ext cx="2521080" cy="1479626"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1753,32 +2181,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U21"/>
+  <dimension ref="A1:U65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:K21"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="4.109375" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" customWidth="1"/>
-    <col min="4" max="4" width="3.77734375" customWidth="1"/>
-    <col min="5" max="5" width="7.109375" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" customWidth="1"/>
-    <col min="7" max="7" width="11.77734375" customWidth="1"/>
-    <col min="8" max="8" width="3.88671875" customWidth="1"/>
+    <col min="1" max="1" width="4.08984375" customWidth="1"/>
+    <col min="2" max="2" width="15.453125" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" customWidth="1"/>
+    <col min="4" max="4" width="3.81640625" customWidth="1"/>
+    <col min="5" max="5" width="7.08984375" customWidth="1"/>
+    <col min="6" max="6" width="11.6328125" customWidth="1"/>
+    <col min="7" max="7" width="11.81640625" customWidth="1"/>
+    <col min="8" max="8" width="3.90625" customWidth="1"/>
     <col min="9" max="9" width="5" customWidth="1"/>
-    <col min="10" max="10" width="12.88671875" customWidth="1"/>
-    <col min="11" max="11" width="12.5546875" customWidth="1"/>
-    <col min="12" max="12" width="3.33203125" customWidth="1"/>
-    <col min="16" max="16" width="3.109375" customWidth="1"/>
-    <col min="17" max="17" width="4.109375" customWidth="1"/>
-    <col min="18" max="18" width="3.5546875" customWidth="1"/>
-    <col min="19" max="20" width="3.6640625" customWidth="1"/>
-    <col min="21" max="21" width="4.6640625" customWidth="1"/>
-    <col min="22" max="22" width="3.6640625" customWidth="1"/>
+    <col min="10" max="10" width="12.90625" customWidth="1"/>
+    <col min="11" max="11" width="12.54296875" customWidth="1"/>
+    <col min="12" max="12" width="3.36328125" customWidth="1"/>
+    <col min="16" max="16" width="3.08984375" customWidth="1"/>
+    <col min="17" max="17" width="4.08984375" customWidth="1"/>
+    <col min="18" max="18" width="3.54296875" customWidth="1"/>
+    <col min="19" max="20" width="3.6328125" customWidth="1"/>
+    <col min="21" max="21" width="4.6328125" customWidth="1"/>
+    <col min="22" max="22" width="3.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
@@ -1804,123 +2232,123 @@
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
     </row>
-    <row r="3" spans="1:21" ht="18">
-      <c r="A3" s="48" t="s">
+    <row r="3" spans="1:21" ht="18.5">
+      <c r="A3" s="91" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="E3" s="52" t="s">
+      <c r="B3" s="91"/>
+      <c r="C3" s="91"/>
+      <c r="E3" s="87" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="88"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="54" t="s">
+      <c r="I3" s="82" t="s">
         <v>42</v>
       </c>
-      <c r="J3" s="55"/>
-      <c r="K3" s="56"/>
-    </row>
-    <row r="4" spans="1:21" ht="37.200000000000003" customHeight="1">
-      <c r="A4" s="85" t="s">
+      <c r="J3" s="83"/>
+      <c r="K3" s="84"/>
+    </row>
+    <row r="4" spans="1:21" ht="37.25" customHeight="1">
+      <c r="A4" s="89" t="s">
         <v>107</v>
       </c>
-      <c r="B4" s="86"/>
+      <c r="B4" s="90"/>
       <c r="C4" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="49" t="s">
+      <c r="E4" s="92" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="50"/>
-      <c r="G4" s="74" t="s">
+      <c r="F4" s="93"/>
+      <c r="G4" s="64" t="s">
         <v>108</v>
       </c>
       <c r="H4" s="10"/>
-      <c r="I4" s="77" t="s">
+      <c r="I4" s="85" t="s">
         <v>110</v>
       </c>
-      <c r="J4" s="78"/>
-      <c r="K4" s="81" t="s">
+      <c r="J4" s="86"/>
+      <c r="K4" s="69" t="s">
         <v>43</v>
       </c>
       <c r="M4" s="2"/>
     </row>
     <row r="5" spans="1:21">
-      <c r="A5" s="82" t="s">
+      <c r="A5" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="82" t="s">
+      <c r="B5" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="83" t="s">
+      <c r="C5" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="72" t="s">
+      <c r="E5" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="72" t="s">
+      <c r="F5" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="73" t="s">
+      <c r="G5" s="63" t="s">
         <v>0</v>
       </c>
       <c r="H5" s="11"/>
-      <c r="I5" s="79" t="s">
+      <c r="I5" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="J5" s="79" t="s">
+      <c r="J5" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="K5" s="82" t="s">
+      <c r="K5" s="70" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:21">
-      <c r="A6" s="80">
+      <c r="A6" s="68">
         <v>20</v>
       </c>
-      <c r="B6" s="84" t="s">
+      <c r="B6" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="36">
+      <c r="C6" s="35">
         <v>39</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="35">
         <v>39</v>
       </c>
-      <c r="F6" s="37" t="s">
+      <c r="F6" s="36" t="s">
         <v>56</v>
       </c>
       <c r="G6" s="9">
         <v>37</v>
       </c>
       <c r="H6" s="12"/>
-      <c r="I6" s="75">
+      <c r="I6" s="65">
         <v>38</v>
       </c>
-      <c r="J6" s="76" t="s">
+      <c r="J6" s="66" t="s">
         <v>52</v>
       </c>
-      <c r="K6" s="80" t="s">
+      <c r="K6" s="68" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:21">
-      <c r="A7" s="57">
+      <c r="A7" s="48">
         <v>21</v>
       </c>
-      <c r="B7" s="64" t="s">
+      <c r="B7" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="36">
+      <c r="C7" s="35">
         <v>41</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="35">
         <v>41</v>
       </c>
-      <c r="F7" s="37" t="s">
+      <c r="F7" s="36" t="s">
         <v>55</v>
       </c>
       <c r="G7" s="9">
@@ -1933,24 +2361,24 @@
       <c r="J7" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="K7" s="57" t="s">
+      <c r="K7" s="48" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:21">
-      <c r="A8" s="57">
+      <c r="A8" s="48">
         <v>17</v>
       </c>
-      <c r="B8" s="65" t="s">
+      <c r="B8" s="55" t="s">
         <v>121</v>
       </c>
-      <c r="C8" s="36">
+      <c r="C8" s="35">
         <v>45</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="35">
         <v>45</v>
       </c>
-      <c r="F8" s="37" t="s">
+      <c r="F8" s="36" t="s">
         <v>44</v>
       </c>
       <c r="G8" s="9">
@@ -1963,25 +2391,25 @@
       <c r="J8" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="K8" s="57" t="s">
+      <c r="K8" s="48" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="28.8">
-      <c r="A9" s="57">
+    <row r="9" spans="1:21" ht="29">
+      <c r="A9" s="48">
         <v>18</v>
       </c>
-      <c r="B9" s="66" t="s">
+      <c r="B9" s="56" t="s">
         <v>120</v>
       </c>
-      <c r="C9" s="36">
+      <c r="C9" s="35">
         <v>47</v>
       </c>
       <c r="D9" s="1"/>
-      <c r="E9" s="36">
+      <c r="E9" s="35">
         <v>47</v>
       </c>
-      <c r="F9" s="37" t="s">
+      <c r="F9" s="36" t="s">
         <v>45</v>
       </c>
       <c r="G9" s="9">
@@ -1994,25 +2422,25 @@
       <c r="J9" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="K9" s="57" t="s">
+      <c r="K9" s="48" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:21">
-      <c r="A10" s="58">
+      <c r="A10" s="49">
         <v>9</v>
       </c>
-      <c r="B10" s="67" t="s">
+      <c r="B10" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="C10" s="38">
+      <c r="C10" s="37">
         <v>40</v>
       </c>
       <c r="D10" s="13"/>
-      <c r="E10" s="38">
+      <c r="E10" s="37">
         <v>40</v>
       </c>
-      <c r="F10" s="39" t="s">
+      <c r="F10" s="38" t="s">
         <v>10</v>
       </c>
       <c r="G10" s="14">
@@ -2025,25 +2453,25 @@
       <c r="J10" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="K10" s="58" t="s">
+      <c r="K10" s="49" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:21">
-      <c r="A11" s="58">
+      <c r="A11" s="49">
         <v>8</v>
       </c>
-      <c r="B11" s="67" t="s">
+      <c r="B11" s="57" t="s">
         <v>60</v>
       </c>
-      <c r="C11" s="38">
+      <c r="C11" s="37">
         <v>38</v>
       </c>
       <c r="D11" s="13"/>
-      <c r="E11" s="38">
+      <c r="E11" s="37">
         <v>38</v>
       </c>
-      <c r="F11" s="39" t="s">
+      <c r="F11" s="38" t="s">
         <v>12</v>
       </c>
       <c r="G11" s="14">
@@ -2056,25 +2484,25 @@
       <c r="J11" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="K11" s="58" t="s">
+      <c r="K11" s="49" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:21">
-      <c r="A12" s="57">
+      <c r="A12" s="48">
         <v>3</v>
       </c>
-      <c r="B12" s="68" t="s">
+      <c r="B12" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="41">
+      <c r="C12" s="40">
         <v>21</v>
       </c>
       <c r="D12" s="17"/>
-      <c r="E12" s="41">
+      <c r="E12" s="40">
         <v>21</v>
       </c>
-      <c r="F12" s="40" t="s">
+      <c r="F12" s="39" t="s">
         <v>4</v>
       </c>
       <c r="G12" s="18">
@@ -2087,25 +2515,25 @@
       <c r="J12" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="K12" s="59" t="s">
+      <c r="K12" s="50" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:21">
-      <c r="A13" s="57">
+      <c r="A13" s="48">
         <v>2</v>
       </c>
-      <c r="B13" s="68" t="s">
+      <c r="B13" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="41">
+      <c r="C13" s="40">
         <v>23</v>
       </c>
       <c r="D13" s="17"/>
-      <c r="E13" s="41">
+      <c r="E13" s="40">
         <v>23</v>
       </c>
-      <c r="F13" s="40" t="s">
+      <c r="F13" s="39" t="s">
         <v>7</v>
       </c>
       <c r="G13" s="18">
@@ -2118,25 +2546,25 @@
       <c r="J13" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="K13" s="59" t="s">
+      <c r="K13" s="50" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:21">
-      <c r="A14" s="60">
+      <c r="A14" s="51">
         <v>6</v>
       </c>
-      <c r="B14" s="69" t="s">
+      <c r="B14" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="42">
+      <c r="C14" s="41">
         <v>16</v>
       </c>
       <c r="D14" s="21"/>
-      <c r="E14" s="42">
+      <c r="E14" s="41">
         <v>16</v>
       </c>
-      <c r="F14" s="43" t="s">
+      <c r="F14" s="42" t="s">
         <v>17</v>
       </c>
       <c r="G14" s="22">
@@ -2149,25 +2577,25 @@
       <c r="J14" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="K14" s="60" t="s">
+      <c r="K14" s="51" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:21">
-      <c r="A15" s="60">
+      <c r="A15" s="51">
         <v>5</v>
       </c>
-      <c r="B15" s="69" t="s">
+      <c r="B15" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="42">
+      <c r="C15" s="41">
         <v>14</v>
       </c>
       <c r="D15" s="21"/>
-      <c r="E15" s="42">
+      <c r="E15" s="41">
         <v>14</v>
       </c>
-      <c r="F15" s="43" t="s">
+      <c r="F15" s="42" t="s">
         <v>21</v>
       </c>
       <c r="G15" s="22">
@@ -2180,25 +2608,25 @@
       <c r="J15" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="K15" s="60" t="s">
+      <c r="K15" s="51" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:21">
-      <c r="A16" s="61">
+      <c r="A16" s="52">
         <v>12</v>
       </c>
-      <c r="B16" s="70" t="s">
+      <c r="B16" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="44">
+      <c r="C16" s="43">
         <v>22</v>
       </c>
       <c r="D16" s="25"/>
-      <c r="E16" s="44">
+      <c r="E16" s="43">
         <v>22</v>
       </c>
-      <c r="F16" s="45" t="s">
+      <c r="F16" s="44" t="s">
         <v>25</v>
       </c>
       <c r="G16" s="26">
@@ -2211,25 +2639,25 @@
       <c r="J16" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="K16" s="61" t="s">
+      <c r="K16" s="52" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="61">
+      <c r="A17" s="52">
         <v>11</v>
       </c>
-      <c r="B17" s="70" t="s">
+      <c r="B17" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="44">
+      <c r="C17" s="43">
         <v>20</v>
       </c>
       <c r="D17" s="25"/>
-      <c r="E17" s="44">
+      <c r="E17" s="43">
         <v>20</v>
       </c>
-      <c r="F17" s="45" t="s">
+      <c r="F17" s="44" t="s">
         <v>29</v>
       </c>
       <c r="G17" s="26">
@@ -2242,25 +2670,25 @@
       <c r="J17" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="K17" s="61" t="s">
+      <c r="K17" s="52" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="62">
+      <c r="A18" s="53">
         <v>15</v>
       </c>
-      <c r="B18" s="71" t="s">
+      <c r="B18" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="46">
+      <c r="C18" s="45">
         <v>32</v>
       </c>
       <c r="D18" s="29"/>
-      <c r="E18" s="46">
+      <c r="E18" s="45">
         <v>32</v>
       </c>
-      <c r="F18" s="47" t="s">
+      <c r="F18" s="46" t="s">
         <v>33</v>
       </c>
       <c r="G18" s="30">
@@ -2273,25 +2701,25 @@
       <c r="J18" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="K18" s="62" t="s">
+      <c r="K18" s="53" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="62">
+      <c r="A19" s="53">
         <v>14</v>
       </c>
-      <c r="B19" s="71" t="s">
+      <c r="B19" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="46">
+      <c r="C19" s="45">
         <v>34</v>
       </c>
       <c r="D19" s="29"/>
-      <c r="E19" s="46">
+      <c r="E19" s="45">
         <v>34</v>
       </c>
-      <c r="F19" s="47" t="s">
+      <c r="F19" s="46" t="s">
         <v>37</v>
       </c>
       <c r="G19" s="30">
@@ -2304,39 +2732,112 @@
       <c r="J19" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="K19" s="62" t="s">
+      <c r="K19" s="53" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="3"/>
-      <c r="D20" s="51" t="s">
+      <c r="A20" s="53"/>
+      <c r="B20" s="61"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="53"/>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="53"/>
+      <c r="B21" s="61"/>
+      <c r="C21" s="45">
+        <v>36</v>
+      </c>
+      <c r="D21" s="29"/>
+      <c r="E21" s="45">
+        <v>36</v>
+      </c>
+      <c r="F21" s="46" t="s">
+        <v>125</v>
+      </c>
+      <c r="G21" s="30">
+        <v>8</v>
+      </c>
+      <c r="H21" s="31"/>
+      <c r="I21" s="30">
+        <v>7</v>
+      </c>
+      <c r="J21" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="K21" s="53"/>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="53"/>
+      <c r="B22" s="61"/>
+      <c r="C22" s="45">
+        <v>36</v>
+      </c>
+      <c r="D22" s="29"/>
+      <c r="E22" s="45">
+        <v>36</v>
+      </c>
+      <c r="F22" s="46" t="s">
+        <v>125</v>
+      </c>
+      <c r="G22" s="30">
+        <v>10</v>
+      </c>
+      <c r="H22" s="31"/>
+      <c r="I22" s="30">
+        <v>9</v>
+      </c>
+      <c r="J22" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="K22" s="53"/>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" s="3"/>
+      <c r="D23" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="H20" s="51" t="s">
+      <c r="H23" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="K20" s="95" t="s">
+      <c r="K23" s="78" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="83.4" customHeight="1">
-      <c r="A21" s="94" t="s">
+    <row r="24" spans="1:11" ht="55.5" customHeight="1">
+      <c r="A24" s="81" t="s">
         <v>123</v>
       </c>
-      <c r="B21" s="94"/>
-      <c r="C21" s="94"/>
-      <c r="G21" s="92" t="s">
+      <c r="B24" s="81"/>
+      <c r="C24" s="81"/>
+      <c r="G24" s="79" t="s">
         <v>118</v>
       </c>
-      <c r="H21" s="93"/>
-      <c r="I21" s="93"/>
-      <c r="J21" s="93"/>
+      <c r="H24" s="80"/>
+      <c r="I24" s="80"/>
+      <c r="J24" s="80"/>
+    </row>
+    <row r="50" spans="2:2" ht="25.5" customHeight="1">
+      <c r="B50" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2">
+      <c r="B65" t="s">
+        <v>129</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="G21:J21"/>
-    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="G24:J24"/>
+    <mergeCell ref="A24:C24"/>
     <mergeCell ref="I3:K3"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="E3:G3"/>
@@ -2346,31 +2847,32 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:L59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="5.21875" customWidth="1"/>
+    <col min="1" max="1" width="5.1796875" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="4.21875" customWidth="1"/>
-    <col min="4" max="4" width="7.77734375" customWidth="1"/>
-    <col min="5" max="5" width="3.77734375" customWidth="1"/>
-    <col min="6" max="6" width="4.21875" customWidth="1"/>
-    <col min="7" max="7" width="11.109375" customWidth="1"/>
-    <col min="8" max="8" width="11.5546875" customWidth="1"/>
-    <col min="9" max="9" width="3.44140625" customWidth="1"/>
-    <col min="10" max="10" width="6.109375" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" customWidth="1"/>
-    <col min="12" max="12" width="10.6640625" customWidth="1"/>
+    <col min="3" max="3" width="4.1796875" customWidth="1"/>
+    <col min="4" max="4" width="7.81640625" customWidth="1"/>
+    <col min="5" max="5" width="3.81640625" customWidth="1"/>
+    <col min="6" max="6" width="4.1796875" customWidth="1"/>
+    <col min="7" max="7" width="11.08984375" customWidth="1"/>
+    <col min="8" max="8" width="11.54296875" customWidth="1"/>
+    <col min="9" max="9" width="3.453125" customWidth="1"/>
+    <col min="10" max="10" width="6.08984375" customWidth="1"/>
+    <col min="11" max="11" width="14.36328125" customWidth="1"/>
+    <col min="12" max="12" width="10.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -2378,113 +2880,113 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="18">
-      <c r="A3" s="63" t="s">
+    <row r="3" spans="1:12" ht="18.5">
+      <c r="A3" s="95" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="63"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="F3" s="52" t="s">
+      <c r="B3" s="95"/>
+      <c r="C3" s="95"/>
+      <c r="D3" s="95"/>
+      <c r="F3" s="87" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
+      <c r="G3" s="88"/>
+      <c r="H3" s="88"/>
       <c r="I3" s="10"/>
-      <c r="J3" s="54" t="s">
+      <c r="J3" s="82" t="s">
         <v>42</v>
       </c>
-      <c r="K3" s="55"/>
-      <c r="L3" s="56"/>
-    </row>
-    <row r="4" spans="1:12" ht="37.799999999999997" customHeight="1">
-      <c r="A4" s="85" t="s">
+      <c r="K3" s="83"/>
+      <c r="L3" s="84"/>
+    </row>
+    <row r="4" spans="1:12" ht="37.75" customHeight="1">
+      <c r="A4" s="89" t="s">
         <v>119</v>
       </c>
-      <c r="B4" s="85"/>
-      <c r="C4" s="35" t="s">
+      <c r="B4" s="89"/>
+      <c r="C4" s="94" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="35"/>
-      <c r="F4" s="49" t="s">
+      <c r="D4" s="94"/>
+      <c r="F4" s="92" t="s">
         <v>61</v>
       </c>
-      <c r="G4" s="50"/>
-      <c r="H4" s="74" t="s">
+      <c r="G4" s="93"/>
+      <c r="H4" s="64" t="s">
         <v>115</v>
       </c>
       <c r="I4" s="10"/>
-      <c r="J4" s="77" t="s">
+      <c r="J4" s="85" t="s">
         <v>116</v>
       </c>
-      <c r="K4" s="78"/>
-      <c r="L4" s="81" t="s">
+      <c r="K4" s="86"/>
+      <c r="L4" s="69" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="82" t="s">
+      <c r="A5" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="82" t="s">
+      <c r="B5" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="91" t="s">
+      <c r="C5" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="91" t="s">
+      <c r="D5" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="72" t="s">
+      <c r="F5" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="72" t="s">
+      <c r="G5" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="73" t="s">
+      <c r="H5" s="63" t="s">
         <v>0</v>
       </c>
       <c r="I5" s="11"/>
-      <c r="J5" s="79" t="s">
+      <c r="J5" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="K5" s="79" t="s">
+      <c r="K5" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="L5" s="82" t="s">
+      <c r="L5" s="70" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="87">
+      <c r="A6" s="73">
         <v>3</v>
       </c>
-      <c r="B6" s="88" t="s">
+      <c r="B6" s="74" t="s">
         <v>90</v>
       </c>
-      <c r="C6" s="89">
+      <c r="C6" s="75">
         <v>17</v>
       </c>
-      <c r="D6" s="90" t="s">
+      <c r="D6" s="76" t="s">
         <v>98</v>
       </c>
-      <c r="F6" s="36">
+      <c r="F6" s="35">
         <v>17</v>
       </c>
-      <c r="G6" s="37" t="s">
+      <c r="G6" s="36" t="s">
         <v>79</v>
       </c>
       <c r="H6" s="9">
         <v>56</v>
       </c>
       <c r="I6" s="12"/>
-      <c r="J6" s="75">
+      <c r="J6" s="65">
         <v>55</v>
       </c>
-      <c r="K6" s="76" t="s">
+      <c r="K6" s="66" t="s">
         <v>71</v>
       </c>
-      <c r="L6" s="80" t="s">
+      <c r="L6" s="68" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2495,16 +2997,16 @@
       <c r="B7" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C7" s="36">
+      <c r="C7" s="35">
         <v>15</v>
       </c>
-      <c r="D7" s="37" t="s">
+      <c r="D7" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="F7" s="36">
+      <c r="F7" s="35">
         <v>15</v>
       </c>
-      <c r="G7" s="37" t="s">
+      <c r="G7" s="36" t="s">
         <v>80</v>
       </c>
       <c r="H7" s="9">
@@ -2517,7 +3019,7 @@
       <c r="K7" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="L7" s="57" t="s">
+      <c r="L7" s="48" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2528,16 +3030,16 @@
       <c r="B8" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C8" s="36">
+      <c r="C8" s="35">
         <v>40</v>
       </c>
-      <c r="D8" s="37" t="s">
+      <c r="D8" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="F8" s="36">
+      <c r="F8" s="35">
         <v>40</v>
       </c>
-      <c r="G8" s="37" t="s">
+      <c r="G8" s="36" t="s">
         <v>81</v>
       </c>
       <c r="H8" s="9">
@@ -2550,7 +3052,7 @@
       <c r="K8" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="L8" s="57" t="s">
+      <c r="L8" s="48" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2561,17 +3063,17 @@
       <c r="B9" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="C9" s="38">
+      <c r="C9" s="37">
         <v>29</v>
       </c>
-      <c r="D9" s="39" t="s">
+      <c r="D9" s="38" t="s">
         <v>100</v>
       </c>
       <c r="E9" s="13"/>
-      <c r="F9" s="38">
+      <c r="F9" s="37">
         <v>29</v>
       </c>
-      <c r="G9" s="39" t="s">
+      <c r="G9" s="38" t="s">
         <v>83</v>
       </c>
       <c r="H9" s="14">
@@ -2584,7 +3086,7 @@
       <c r="K9" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="L9" s="58" t="s">
+      <c r="L9" s="49" t="s">
         <v>113</v>
       </c>
     </row>
@@ -2595,17 +3097,17 @@
       <c r="B10" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="C10" s="38">
+      <c r="C10" s="37">
         <v>27</v>
       </c>
-      <c r="D10" s="39" t="s">
+      <c r="D10" s="38" t="s">
         <v>101</v>
       </c>
       <c r="E10" s="13"/>
-      <c r="F10" s="38">
+      <c r="F10" s="37">
         <v>27</v>
       </c>
-      <c r="G10" s="39" t="s">
+      <c r="G10" s="38" t="s">
         <v>82</v>
       </c>
       <c r="H10" s="14">
@@ -2618,7 +3120,7 @@
       <c r="K10" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="L10" s="58" t="s">
+      <c r="L10" s="49" t="s">
         <v>114</v>
       </c>
     </row>
@@ -2629,17 +3131,17 @@
       <c r="B11" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C11" s="41">
+      <c r="C11" s="40">
         <v>33</v>
       </c>
-      <c r="D11" s="40" t="s">
+      <c r="D11" s="39" t="s">
         <v>102</v>
       </c>
       <c r="E11" s="17"/>
-      <c r="F11" s="41">
+      <c r="F11" s="40">
         <v>33</v>
       </c>
-      <c r="G11" s="40" t="s">
+      <c r="G11" s="39" t="s">
         <v>84</v>
       </c>
       <c r="H11" s="18">
@@ -2652,7 +3154,7 @@
       <c r="K11" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="L11" s="59" t="s">
+      <c r="L11" s="50" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2663,17 +3165,17 @@
       <c r="B12" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C12" s="41">
+      <c r="C12" s="40">
         <v>35</v>
       </c>
-      <c r="D12" s="40" t="s">
+      <c r="D12" s="39" t="s">
         <v>103</v>
       </c>
       <c r="E12" s="17"/>
-      <c r="F12" s="41">
+      <c r="F12" s="40">
         <v>35</v>
       </c>
-      <c r="G12" s="40" t="s">
+      <c r="G12" s="39" t="s">
         <v>85</v>
       </c>
       <c r="H12" s="18">
@@ -2686,7 +3188,7 @@
       <c r="K12" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="L12" s="59" t="s">
+      <c r="L12" s="50" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2697,17 +3199,17 @@
       <c r="B13" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C13" s="42">
+      <c r="C13" s="41">
         <v>41</v>
       </c>
-      <c r="D13" s="43" t="s">
+      <c r="D13" s="42" t="s">
         <v>104</v>
       </c>
       <c r="E13" s="21"/>
-      <c r="F13" s="42">
+      <c r="F13" s="41">
         <v>41</v>
       </c>
-      <c r="G13" s="43" t="s">
+      <c r="G13" s="42" t="s">
         <v>86</v>
       </c>
       <c r="H13" s="22">
@@ -2720,7 +3222,7 @@
       <c r="K13" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="L13" s="60" t="s">
+      <c r="L13" s="51" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2731,17 +3233,17 @@
       <c r="B14" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C14" s="42">
+      <c r="C14" s="41">
         <v>39</v>
       </c>
-      <c r="D14" s="43" t="s">
+      <c r="D14" s="42" t="s">
         <v>105</v>
       </c>
       <c r="E14" s="21"/>
-      <c r="F14" s="42">
+      <c r="F14" s="41">
         <v>39</v>
       </c>
-      <c r="G14" s="43" t="s">
+      <c r="G14" s="42" t="s">
         <v>87</v>
       </c>
       <c r="H14" s="22">
@@ -2754,32 +3256,108 @@
       <c r="K14" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="L14" s="60" t="s">
+      <c r="L14" s="51" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="E15" s="51" t="s">
+      <c r="A15" s="8"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="51"/>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="8"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="41">
+        <v>36</v>
+      </c>
+      <c r="D16" s="42"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="41">
+        <v>36</v>
+      </c>
+      <c r="G16" s="42" t="s">
+        <v>127</v>
+      </c>
+      <c r="H16" s="22">
+        <v>10</v>
+      </c>
+      <c r="I16" s="23"/>
+      <c r="J16" s="22">
+        <v>9</v>
+      </c>
+      <c r="K16" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="L16" s="51"/>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="8"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="41">
+        <v>36</v>
+      </c>
+      <c r="D17" s="42"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="41">
+        <v>36</v>
+      </c>
+      <c r="G17" s="42" t="s">
+        <v>127</v>
+      </c>
+      <c r="H17" s="22">
+        <v>12</v>
+      </c>
+      <c r="I17" s="23"/>
+      <c r="J17" s="22">
+        <v>11</v>
+      </c>
+      <c r="K17" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="L17" s="51"/>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="E18" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="I15" s="51" t="s">
+      <c r="I18" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="L15" s="95" t="s">
+      <c r="L18" s="78" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="55.2" customHeight="1">
-      <c r="H16" s="92" t="s">
+    <row r="19" spans="1:12" ht="55.25" customHeight="1">
+      <c r="H19" s="79" t="s">
         <v>118</v>
       </c>
-      <c r="I16" s="93"/>
-      <c r="J16" s="93"/>
-      <c r="K16" s="93"/>
+      <c r="I19" s="80"/>
+      <c r="J19" s="80"/>
+      <c r="K19" s="80"/>
+    </row>
+    <row r="45" spans="2:2" ht="25.5" customHeight="1">
+      <c r="B45" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2">
+      <c r="B59" t="s">
+        <v>129</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="H19:K19"/>
     <mergeCell ref="F3:H3"/>
     <mergeCell ref="J3:L3"/>
     <mergeCell ref="C4:D4"/>
@@ -2789,5 +3367,6 @@
     <mergeCell ref="A4:B4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added power-related CRUVI info.
</commit_message>
<xml_diff>
--- a/0.doc/CRUVI-camera-adapter/CRUVI-Pinout-4-and-2-lanes.xlsx
+++ b/0.doc/CRUVI-camera-adapter/CRUVI-Pinout-4-and-2-lanes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="310" windowWidth="15010" windowHeight="8220" activeTab="1"/>
+    <workbookView xWindow="400" yWindow="310" windowWidth="15010" windowHeight="8220" tabRatio="460"/>
   </bookViews>
   <sheets>
     <sheet name="4 Lanes" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="141">
   <si>
     <t>pin</t>
   </si>
@@ -435,10 +435,6 @@
     </r>
   </si>
   <si>
-    <t>These 2 connectors are hermaphroditic. ODD pin numbers on the SOM are connected to EVEN pin
-numbers on the Carrier, and vice versa</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">From Camera
 </t>
@@ -463,6 +459,96 @@
   </si>
   <si>
     <t>VADJ or 3.3V</t>
+  </si>
+  <si>
+    <t>VCCIO35</t>
+  </si>
+  <si>
+    <t>VCCIO_CA</t>
+  </si>
+  <si>
+    <t>VCCIO15</t>
+  </si>
+  <si>
+    <t>VCCIO_CC</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>VS0, 1, 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> come from CPLD. Default RTL provides 1.8V and 2.5V:</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">FPGA IBUFDS, to be LVDS, can only work with 2.5V (LVDS_25) and 1.8V VCCO (LVDS) </t>
+  </si>
+  <si>
+    <t>VADJ (not used)</t>
+  </si>
+  <si>
+    <t>on-board 100ohm terminaton resistors (0402)</t>
+  </si>
+  <si>
+    <t>https://support.xilinx.com/s/article/43989?language=en_US</t>
+  </si>
+  <si>
+    <t>3.3V</t>
+  </si>
+  <si>
+    <t>3.3V supply</t>
+  </si>
+  <si>
+    <t>Carrier side of CRUVI</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">These 2 connectors are hermaphroditic. ODD pin numbers on the SOM are connected to EVEN pin
+numbers on the Carrier, and vice versa. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Also note P/N inversion on most of differential signals!</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">These 2 connectors are hermaphroditic. ODD pin numbers on the SOM are connected to EVEN pin. 
+numbers on the Carrier, and vice versa. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Also note P/N inversion on most of differential signals!</t>
+    </r>
   </si>
   <si>
     <r>
@@ -486,54 +572,38 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> 
-1) Camera I2C is kept separately from I2C for CRUVI-optional ID EEPROM
-2) Pay attention to voltage levels between FPGA (VADJ) and Camera I2C and POWER_EN, which are 3.3V</t>
+</t>
     </r>
-  </si>
-  <si>
-    <t>VCCIO35</t>
-  </si>
-  <si>
-    <t>VCCIO_CA</t>
-  </si>
-  <si>
-    <t>VCCIO15</t>
-  </si>
-  <si>
-    <t>VCCIO_CC</t>
-  </si>
-  <si>
     <r>
       <rPr>
-        <b/>
-        <sz val="11"/>
+        <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>VS0, 1, 2</t>
+      <t>1) Camera I2C is kept separately from I2C for CRUVI-optional ID EEPROM
+2) Pay attention to voltage levels between FPGA (VADJ) and Camera I2C and POWER_EN, which are 3.3V</t>
     </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> come from CPLD. Default RTL provides 1.8V and 2.5V:</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">FPGA IBUFDS, to be LVDS, can only work with 2.5V (LVDS_25) and 1.8V VCCO (LVDS) </t>
+  </si>
+  <si>
+    <t>4, 9</t>
+  </si>
+  <si>
+    <t>GND</t>
+  </si>
+  <si>
+    <t>multiple</t>
+  </si>
+  <si>
+    <t>https://www.arducam.com/raspberry-pi-camera-pinout/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="27">
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -731,6 +801,28 @@
       <b/>
       <u/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1162,7 +1254,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1205,8 +1297,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1451,8 +1547,14 @@
     <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="42" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="2" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="3" builtinId="38" customBuiltin="1"/>
@@ -1486,6 +1588,7 @@
     <cellStyle name="Heading 2" xfId="31" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="32" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="33" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="34" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="35" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="36" builtinId="28" customBuiltin="1"/>
@@ -1512,13 +1615,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>38099</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>311150</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>6766</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1550,13 +1653,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>107950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>533662</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>158781</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1588,13 +1691,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>520700</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>768541</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>44550</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1626,13 +1729,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>603250</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>216100</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>65</xdr:row>
       <xdr:rowOff>171565</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1664,13 +1767,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>965200</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>25530</xdr:colOff>
-      <xdr:row>74</xdr:row>
+      <xdr:row>77</xdr:row>
       <xdr:rowOff>76</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1698,6 +1801,196 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7" descr="LVDS_25.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="285750" y="15360650"/>
+          <a:ext cx="7791450" cy="5016500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>145</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8" descr="LVDS.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="285750" y="20516850"/>
+          <a:ext cx="7385050" cy="4991100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>489513</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9" descr="LVDS-vs-VCCO.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="292100" y="15786100"/>
+          <a:ext cx="7715813" cy="1803400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>508217</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>146236</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10" descr="Carrier-side-of-CRUVI.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7473950" y="6540500"/>
+          <a:ext cx="4216617" cy="3613336"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>50799</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>152908</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7518400" y="419099"/>
+          <a:ext cx="2940050" cy="4674109"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1707,13 +2000,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>222250</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>603250</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>132260</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1744,19 +2037,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>120650</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
+      <xdr:colOff>8467</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>876562</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>158781</xdr:rowOff>
+      <xdr:colOff>838201</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>119063</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="8" name="Picture 7" descr="VHDPlus-100ohm-termination.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1769,8 +2062,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="482600" y="6305550"/>
-          <a:ext cx="5099312" cy="603281"/>
+          <a:off x="370417" y="14541500"/>
+          <a:ext cx="5916084" cy="4437063"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1781,20 +2074,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>82741</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>120750</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>606974</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>27318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPr id="9" name="Picture 8" descr="VHDPlus-CRUVI.2-lane.15pin.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1807,8 +2100,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1079500" y="6959600"/>
-          <a:ext cx="3708591" cy="1936850"/>
+          <a:off x="381000" y="11982450"/>
+          <a:ext cx="17783724" cy="9158618"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1819,20 +2112,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>654050</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>82550</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>565150</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>84438</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>209750</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>114415</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>41969</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPr id="11" name="Picture 10"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1845,46 +2138,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1016000" y="9226550"/>
-          <a:ext cx="3899100" cy="2241665"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>44450</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>685930</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>76</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1397000" y="12039600"/>
-          <a:ext cx="2521080" cy="1479626"/>
+          <a:off x="7346950" y="452738"/>
+          <a:ext cx="3130550" cy="3615131"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2181,15 +2436,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U65"/>
+  <dimension ref="A1:U79"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O96" sqref="O96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="4.08984375" customWidth="1"/>
+    <col min="1" max="1" width="7.08984375" customWidth="1"/>
     <col min="2" max="2" width="15.453125" customWidth="1"/>
     <col min="3" max="3" width="11.54296875" customWidth="1"/>
     <col min="4" max="4" width="3.81640625" customWidth="1"/>
@@ -2201,6 +2456,7 @@
     <col min="10" max="10" width="12.90625" customWidth="1"/>
     <col min="11" max="11" width="12.54296875" customWidth="1"/>
     <col min="12" max="12" width="3.36328125" customWidth="1"/>
+    <col min="13" max="13" width="4.453125" customWidth="1"/>
     <col min="16" max="16" width="3.08984375" customWidth="1"/>
     <col min="17" max="17" width="4.08984375" customWidth="1"/>
     <col min="18" max="18" width="3.54296875" customWidth="1"/>
@@ -2223,8 +2479,10 @@
     </row>
     <row r="2" spans="1:21">
       <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
+      <c r="N2" s="97" t="s">
+        <v>140</v>
+      </c>
+      <c r="O2" s="3"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
@@ -2370,7 +2628,7 @@
         <v>17</v>
       </c>
       <c r="B8" s="55" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C8" s="35">
         <v>45</v>
@@ -2400,7 +2658,7 @@
         <v>18</v>
       </c>
       <c r="B9" s="56" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C9" s="35">
         <v>47</v>
@@ -2643,7 +2901,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:14">
       <c r="A17" s="52">
         <v>11</v>
       </c>
@@ -2674,7 +2932,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:14">
       <c r="A18" s="53">
         <v>15</v>
       </c>
@@ -2705,7 +2963,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:14">
       <c r="A19" s="53">
         <v>14</v>
       </c>
@@ -2736,7 +2994,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:14">
       <c r="A20" s="53"/>
       <c r="B20" s="61"/>
       <c r="C20" s="45"/>
@@ -2749,95 +3007,166 @@
       <c r="J20" s="32"/>
       <c r="K20" s="53"/>
     </row>
-    <row r="21" spans="1:11">
-      <c r="A21" s="53"/>
-      <c r="B21" s="61"/>
-      <c r="C21" s="45">
+    <row r="21" spans="1:14">
+      <c r="A21" s="53">
+        <v>22</v>
+      </c>
+      <c r="B21" s="61" t="s">
+        <v>131</v>
+      </c>
+      <c r="C21" s="45" t="s">
+        <v>137</v>
+      </c>
+      <c r="D21" s="29"/>
+      <c r="E21" s="45" t="s">
+        <v>137</v>
+      </c>
+      <c r="F21" s="46" t="s">
+        <v>132</v>
+      </c>
+      <c r="G21" s="30"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="53"/>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="53" t="s">
+        <v>139</v>
+      </c>
+      <c r="B22" s="61" t="s">
+        <v>138</v>
+      </c>
+      <c r="C22" s="45" t="s">
+        <v>139</v>
+      </c>
+      <c r="D22" s="29"/>
+      <c r="E22" s="45" t="s">
+        <v>139</v>
+      </c>
+      <c r="F22" s="46" t="s">
+        <v>138</v>
+      </c>
+      <c r="G22" s="30"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="32"/>
+      <c r="K22" s="53"/>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="53"/>
+      <c r="B23" s="61"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="32"/>
+      <c r="K23" s="53"/>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="53"/>
+      <c r="B24" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="C24" s="45">
         <v>36</v>
       </c>
-      <c r="D21" s="29"/>
-      <c r="E21" s="45">
+      <c r="D24" s="29"/>
+      <c r="E24" s="45">
         <v>36</v>
       </c>
-      <c r="F21" s="46" t="s">
-        <v>125</v>
-      </c>
-      <c r="G21" s="30">
+      <c r="F24" s="46" t="s">
+        <v>123</v>
+      </c>
+      <c r="G24" s="30">
         <v>8</v>
       </c>
-      <c r="H21" s="31"/>
-      <c r="I21" s="30">
+      <c r="H24" s="31"/>
+      <c r="I24" s="30">
         <v>7</v>
       </c>
-      <c r="J21" s="32" t="s">
-        <v>124</v>
-      </c>
-      <c r="K21" s="53"/>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="A22" s="53"/>
-      <c r="B22" s="61"/>
-      <c r="C22" s="45">
+      <c r="J24" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="K24" s="53"/>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="53"/>
+      <c r="B25" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="C25" s="45">
         <v>36</v>
       </c>
-      <c r="D22" s="29"/>
-      <c r="E22" s="45">
+      <c r="D25" s="29"/>
+      <c r="E25" s="45">
         <v>36</v>
       </c>
-      <c r="F22" s="46" t="s">
-        <v>125</v>
-      </c>
-      <c r="G22" s="30">
+      <c r="F25" s="46" t="s">
+        <v>123</v>
+      </c>
+      <c r="G25" s="30">
         <v>10</v>
       </c>
-      <c r="H22" s="31"/>
-      <c r="I22" s="30">
+      <c r="H25" s="31"/>
+      <c r="I25" s="30">
         <v>9</v>
       </c>
-      <c r="J22" s="32" t="s">
-        <v>124</v>
-      </c>
-      <c r="K22" s="53"/>
-    </row>
-    <row r="23" spans="1:11">
-      <c r="A23" s="3"/>
-      <c r="D23" s="47" t="s">
+      <c r="J25" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="K25" s="53"/>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" s="3"/>
+      <c r="D26" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="H23" s="47" t="s">
+      <c r="H26" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="K23" s="78" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="55.5" customHeight="1">
-      <c r="A24" s="81" t="s">
-        <v>123</v>
-      </c>
-      <c r="B24" s="81"/>
-      <c r="C24" s="81"/>
-      <c r="G24" s="79" t="s">
-        <v>118</v>
-      </c>
-      <c r="H24" s="80"/>
-      <c r="I24" s="80"/>
-      <c r="J24" s="80"/>
-    </row>
-    <row r="50" spans="2:2" ht="25.5" customHeight="1">
-      <c r="B50" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="65" spans="2:2">
-      <c r="B65" t="s">
-        <v>129</v>
+      <c r="K26" s="78" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="94.5" customHeight="1">
+      <c r="A27" s="81" t="s">
+        <v>136</v>
+      </c>
+      <c r="B27" s="81"/>
+      <c r="C27" s="81"/>
+      <c r="G27" s="79" t="s">
+        <v>134</v>
+      </c>
+      <c r="H27" s="80"/>
+      <c r="I27" s="80"/>
+      <c r="J27" s="80"/>
+      <c r="N27" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" ht="25.5" customHeight="1">
+      <c r="B53" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2">
+      <c r="B68" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2">
+      <c r="B79" s="96" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="G24:J24"/>
-    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="G27:J27"/>
+    <mergeCell ref="A27:C27"/>
     <mergeCell ref="I3:K3"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="E3:G3"/>
@@ -2845,28 +3174,31 @@
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="E4:F4"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B79" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L59"/>
+  <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="5.1796875" customWidth="1"/>
-    <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="4.1796875" customWidth="1"/>
+    <col min="1" max="1" width="7.26953125" customWidth="1"/>
+    <col min="2" max="2" width="14.7265625" customWidth="1"/>
+    <col min="3" max="3" width="7.26953125" customWidth="1"/>
     <col min="4" max="4" width="7.81640625" customWidth="1"/>
     <col min="5" max="5" width="3.81640625" customWidth="1"/>
-    <col min="6" max="6" width="4.1796875" customWidth="1"/>
+    <col min="6" max="6" width="7" customWidth="1"/>
     <col min="7" max="7" width="11.08984375" customWidth="1"/>
     <col min="8" max="8" width="11.54296875" customWidth="1"/>
     <col min="9" max="9" width="3.453125" customWidth="1"/>
@@ -2875,12 +3207,17 @@
     <col min="12" max="12" width="10.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="18.5">
+    <row r="2" spans="1:14">
+      <c r="N2" s="97" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="18.5">
       <c r="A3" s="95" t="s">
         <v>58</v>
       </c>
@@ -2899,9 +3236,9 @@
       <c r="K3" s="83"/>
       <c r="L3" s="84"/>
     </row>
-    <row r="4" spans="1:12" ht="37.75" customHeight="1">
+    <row r="4" spans="1:14" ht="37.75" customHeight="1">
       <c r="A4" s="89" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B4" s="89"/>
       <c r="C4" s="94" t="s">
@@ -2924,7 +3261,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:14">
       <c r="A5" s="70" t="s">
         <v>0</v>
       </c>
@@ -2957,7 +3294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:14">
       <c r="A6" s="73">
         <v>3</v>
       </c>
@@ -2990,7 +3327,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:14">
       <c r="A7" s="8">
         <v>2</v>
       </c>
@@ -3023,7 +3360,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:14">
       <c r="A8" s="8">
         <v>5</v>
       </c>
@@ -3056,7 +3393,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:14">
       <c r="A9" s="33">
         <v>7</v>
       </c>
@@ -3090,7 +3427,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:14">
       <c r="A10" s="33">
         <v>8</v>
       </c>
@@ -3124,7 +3461,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:14">
       <c r="A11" s="8">
         <v>13</v>
       </c>
@@ -3158,7 +3495,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:14">
       <c r="A12" s="8">
         <v>14</v>
       </c>
@@ -3192,7 +3529,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:14">
       <c r="A13" s="8">
         <v>10</v>
       </c>
@@ -3226,7 +3563,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:14">
       <c r="A14" s="8">
         <v>11</v>
       </c>
@@ -3260,7 +3597,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:14">
       <c r="A15" s="8"/>
       <c r="B15" s="4"/>
       <c r="C15" s="41"/>
@@ -3274,90 +3611,151 @@
       <c r="K15" s="24"/>
       <c r="L15" s="51"/>
     </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="8"/>
+    <row r="16" spans="1:14">
+      <c r="A16" s="8">
+        <v>15</v>
+      </c>
       <c r="B16" s="4"/>
-      <c r="C16" s="41">
+      <c r="C16" s="45" t="s">
+        <v>137</v>
+      </c>
+      <c r="D16" s="45" t="s">
+        <v>131</v>
+      </c>
+      <c r="E16" s="21"/>
+      <c r="F16" s="45" t="s">
+        <v>137</v>
+      </c>
+      <c r="G16" s="46" t="s">
+        <v>132</v>
+      </c>
+      <c r="H16" s="22"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="51"/>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="45" t="s">
+        <v>139</v>
+      </c>
+      <c r="D17" s="45" t="s">
+        <v>138</v>
+      </c>
+      <c r="E17" s="21"/>
+      <c r="F17" s="45" t="s">
+        <v>139</v>
+      </c>
+      <c r="G17" s="46" t="s">
+        <v>138</v>
+      </c>
+      <c r="H17" s="22"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="51"/>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="8"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="51"/>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="8"/>
+      <c r="B19" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C19" s="41">
         <v>36</v>
       </c>
-      <c r="D16" s="42"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="41">
+      <c r="D19" s="42"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="41">
         <v>36</v>
       </c>
-      <c r="G16" s="42" t="s">
-        <v>127</v>
-      </c>
-      <c r="H16" s="22">
+      <c r="G19" s="42" t="s">
+        <v>125</v>
+      </c>
+      <c r="H19" s="22">
         <v>10</v>
       </c>
-      <c r="I16" s="23"/>
-      <c r="J16" s="22">
+      <c r="I19" s="23"/>
+      <c r="J19" s="22">
         <v>9</v>
       </c>
-      <c r="K16" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="L16" s="51"/>
-    </row>
-    <row r="17" spans="1:12">
-      <c r="A17" s="8"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="41">
+      <c r="K19" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="L19" s="51"/>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="8"/>
+      <c r="B20" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C20" s="41">
         <v>36</v>
       </c>
-      <c r="D17" s="42"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="41">
+      <c r="D20" s="42"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="41">
         <v>36</v>
       </c>
-      <c r="G17" s="42" t="s">
-        <v>127</v>
-      </c>
-      <c r="H17" s="22">
+      <c r="G20" s="42" t="s">
+        <v>125</v>
+      </c>
+      <c r="H20" s="22">
         <v>12</v>
       </c>
-      <c r="I17" s="23"/>
-      <c r="J17" s="22">
+      <c r="I20" s="23"/>
+      <c r="J20" s="22">
         <v>11</v>
       </c>
-      <c r="K17" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="L17" s="51"/>
-    </row>
-    <row r="18" spans="1:12">
-      <c r="E18" s="47" t="s">
+      <c r="K20" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="L20" s="51"/>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="E21" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="I18" s="47" t="s">
+      <c r="I21" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="L18" s="78" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="55.25" customHeight="1">
-      <c r="H19" s="79" t="s">
-        <v>118</v>
-      </c>
-      <c r="I19" s="80"/>
-      <c r="J19" s="80"/>
-      <c r="K19" s="80"/>
-    </row>
-    <row r="45" spans="2:2" ht="25.5" customHeight="1">
-      <c r="B45" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="59" spans="2:2">
-      <c r="B59" t="s">
+      <c r="L21" s="78" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="90.5" customHeight="1">
+      <c r="H22" s="79" t="s">
+        <v>135</v>
+      </c>
+      <c r="I22" s="80"/>
+      <c r="J22" s="80"/>
+      <c r="K22" s="80"/>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" t="s">
         <v>129</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="H19:K19"/>
+    <mergeCell ref="H22:K22"/>
     <mergeCell ref="F3:H3"/>
     <mergeCell ref="J3:L3"/>
     <mergeCell ref="C4:D4"/>
@@ -3367,6 +3765,7 @@
     <mergeCell ref="A4:B4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added OneInch camera module schematic
</commit_message>
<xml_diff>
--- a/0.doc/CRUVI-camera-adapter/CRUVI-Pinout-4-and-2-lanes.xlsx
+++ b/0.doc/CRUVI-camera-adapter/CRUVI-Pinout-4-and-2-lanes.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="143">
   <si>
     <t>pin</t>
   </si>
@@ -597,6 +597,12 @@
   </si>
   <si>
     <t>https://www.arducam.com/raspberry-pi-camera-pinout/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Also see: </t>
+  </si>
+  <si>
+    <t>https://github.com/will127534/OneInchEye</t>
   </si>
 </sst>
 </file>
@@ -1302,7 +1308,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1496,6 +1502,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="42" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1547,12 +1559,7 @@
     <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="42" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="42" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -2438,8 +2445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O96" sqref="O96"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2479,7 +2486,7 @@
     </row>
     <row r="2" spans="1:21">
       <c r="M2" s="2"/>
-      <c r="N2" s="97" t="s">
+      <c r="N2" s="80" t="s">
         <v>140</v>
       </c>
       <c r="O2" s="3"/>
@@ -2491,43 +2498,43 @@
       <c r="U2" s="2"/>
     </row>
     <row r="3" spans="1:21" ht="18.5">
-      <c r="A3" s="91" t="s">
+      <c r="A3" s="93" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="91"/>
-      <c r="C3" s="91"/>
-      <c r="E3" s="87" t="s">
+      <c r="B3" s="93"/>
+      <c r="C3" s="93"/>
+      <c r="E3" s="89" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="82" t="s">
+      <c r="I3" s="84" t="s">
         <v>42</v>
       </c>
-      <c r="J3" s="83"/>
-      <c r="K3" s="84"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="86"/>
     </row>
     <row r="4" spans="1:21" ht="37.25" customHeight="1">
-      <c r="A4" s="89" t="s">
+      <c r="A4" s="91" t="s">
         <v>107</v>
       </c>
-      <c r="B4" s="90"/>
+      <c r="B4" s="92"/>
       <c r="C4" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="92" t="s">
+      <c r="E4" s="94" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="93"/>
+      <c r="F4" s="95"/>
       <c r="G4" s="64" t="s">
         <v>108</v>
       </c>
       <c r="H4" s="10"/>
-      <c r="I4" s="85" t="s">
+      <c r="I4" s="87" t="s">
         <v>110</v>
       </c>
-      <c r="J4" s="86"/>
+      <c r="J4" s="88"/>
       <c r="K4" s="69" t="s">
         <v>43</v>
       </c>
@@ -2901,7 +2908,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:15">
       <c r="A17" s="52">
         <v>11</v>
       </c>
@@ -2932,7 +2939,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:15">
       <c r="A18" s="53">
         <v>15</v>
       </c>
@@ -2963,7 +2970,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:15">
       <c r="A19" s="53">
         <v>14</v>
       </c>
@@ -2994,7 +3001,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:15">
       <c r="A20" s="53"/>
       <c r="B20" s="61"/>
       <c r="C20" s="45"/>
@@ -3007,7 +3014,7 @@
       <c r="J20" s="32"/>
       <c r="K20" s="53"/>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:15">
       <c r="A21" s="53">
         <v>22</v>
       </c>
@@ -3030,7 +3037,7 @@
       <c r="J21" s="32"/>
       <c r="K21" s="53"/>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:15">
       <c r="A22" s="53" t="s">
         <v>139</v>
       </c>
@@ -3053,7 +3060,7 @@
       <c r="J22" s="32"/>
       <c r="K22" s="53"/>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:15">
       <c r="A23" s="53"/>
       <c r="B23" s="61"/>
       <c r="C23" s="45"/>
@@ -3066,7 +3073,7 @@
       <c r="J23" s="32"/>
       <c r="K23" s="53"/>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:15">
       <c r="A24" s="53"/>
       <c r="B24" s="61" t="s">
         <v>128</v>
@@ -3093,7 +3100,7 @@
       </c>
       <c r="K24" s="53"/>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:15">
       <c r="A25" s="53"/>
       <c r="B25" s="61" t="s">
         <v>128</v>
@@ -3120,7 +3127,7 @@
       </c>
       <c r="K25" s="53"/>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:15">
       <c r="A26" s="3"/>
       <c r="D26" s="47" t="s">
         <v>109</v>
@@ -3131,19 +3138,25 @@
       <c r="K26" s="78" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" ht="94.5" customHeight="1">
-      <c r="A27" s="81" t="s">
+      <c r="N26" t="s">
+        <v>141</v>
+      </c>
+      <c r="O26" s="98" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="94.5" customHeight="1">
+      <c r="A27" s="83" t="s">
         <v>136</v>
       </c>
-      <c r="B27" s="81"/>
-      <c r="C27" s="81"/>
-      <c r="G27" s="79" t="s">
+      <c r="B27" s="83"/>
+      <c r="C27" s="83"/>
+      <c r="G27" s="81" t="s">
         <v>134</v>
       </c>
-      <c r="H27" s="80"/>
-      <c r="I27" s="80"/>
-      <c r="J27" s="80"/>
+      <c r="H27" s="82"/>
+      <c r="I27" s="82"/>
+      <c r="J27" s="82"/>
       <c r="N27" t="s">
         <v>133</v>
       </c>
@@ -3159,7 +3172,7 @@
       </c>
     </row>
     <row r="79" spans="2:2">
-      <c r="B79" s="96" t="s">
+      <c r="B79" s="79" t="s">
         <v>130</v>
       </c>
     </row>
@@ -3176,10 +3189,11 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B79" r:id="rId1"/>
+    <hyperlink ref="O26" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -3213,50 +3227,50 @@
       </c>
     </row>
     <row r="2" spans="1:14">
-      <c r="N2" s="97" t="s">
+      <c r="N2" s="80" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="18.5">
-      <c r="A3" s="95" t="s">
+      <c r="A3" s="97" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="95"/>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
-      <c r="F3" s="87" t="s">
+      <c r="B3" s="97"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="F3" s="89" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="88"/>
-      <c r="H3" s="88"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
       <c r="I3" s="10"/>
-      <c r="J3" s="82" t="s">
+      <c r="J3" s="84" t="s">
         <v>42</v>
       </c>
-      <c r="K3" s="83"/>
-      <c r="L3" s="84"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="86"/>
     </row>
     <row r="4" spans="1:14" ht="37.75" customHeight="1">
-      <c r="A4" s="89" t="s">
+      <c r="A4" s="91" t="s">
         <v>118</v>
       </c>
-      <c r="B4" s="89"/>
-      <c r="C4" s="94" t="s">
+      <c r="B4" s="91"/>
+      <c r="C4" s="96" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="94"/>
-      <c r="F4" s="92" t="s">
+      <c r="D4" s="96"/>
+      <c r="F4" s="94" t="s">
         <v>61</v>
       </c>
-      <c r="G4" s="93"/>
+      <c r="G4" s="95"/>
       <c r="H4" s="64" t="s">
         <v>115</v>
       </c>
       <c r="I4" s="10"/>
-      <c r="J4" s="85" t="s">
+      <c r="J4" s="87" t="s">
         <v>116</v>
       </c>
-      <c r="K4" s="86"/>
+      <c r="K4" s="88"/>
       <c r="L4" s="69" t="s">
         <v>62</v>
       </c>
@@ -3741,12 +3755,12 @@
       </c>
     </row>
     <row r="22" spans="1:12" ht="90.5" customHeight="1">
-      <c r="H22" s="79" t="s">
+      <c r="H22" s="81" t="s">
         <v>135</v>
       </c>
-      <c r="I22" s="80"/>
-      <c r="J22" s="80"/>
-      <c r="K22" s="80"/>
+      <c r="I22" s="82"/>
+      <c r="J22" s="82"/>
+      <c r="K22" s="82"/>
     </row>
     <row r="34" spans="2:2">
       <c r="B34" t="s">

</xml_diff>